<commit_message>
agregada BD lenze comienza estilos en la GUI
</commit_message>
<xml_diff>
--- a/assets/infoplc_net_BH_9300_Servo_controlador_0_37__11kW_v2_1_ES-33-43.xlsx
+++ b/assets/infoplc_net_BH_9300_Servo_controlador_0_37__11kW_v2_1_ES-33-43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivanb\MTO-registro\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD04F64-6F47-41DB-97A7-1B22C77FDFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A9DE50-45B4-4EAF-85D1-FE041007AD88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="6720" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -94,16 +94,6 @@
   <si>
     <r>
       <rPr>
-        <sz val="8.5"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>Caso de corto circuito</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
         <sz val="7"/>
         <rFont val="Lucida Sans Unicode"/>
         <family val="2"/>
@@ -134,16 +124,6 @@
         <family val="2"/>
       </rPr>
       <t>Comprobar cable de motor.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>Corriente de carga capacitiva del cable de motor demasiado alta.</t>
     </r>
   </si>
   <si>
@@ -7214,6 +7194,12 @@
       </rPr>
       <t>P.e. "2091": Una monitorización externa ha generado la advertencia EEr</t>
     </r>
+  </si>
+  <si>
+    <t>Corriente de carga capacitiva del cable de motor demasiado alta.</t>
+  </si>
+  <si>
+    <t>Caso de corto circuito</t>
   </si>
 </sst>
 </file>
@@ -7223,7 +7209,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -7296,6 +7282,12 @@
       <sz val="8"/>
       <name val="Trebuchet MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -7505,7 +7497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -7632,23 +7624,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7659,13 +7645,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -7674,28 +7678,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -7704,22 +7690,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8029,7 +8027,7 @@
   <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75"/>
@@ -8047,10 +8045,10 @@
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="43"/>
+      <c r="C1" s="71"/>
       <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
@@ -8062,35 +8060,35 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A2" s="46">
+    <row r="2" spans="1:7" ht="36" customHeight="1">
+      <c r="A2" s="64">
         <v>11</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="50" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="72" t="s">
+        <v>410</v>
+      </c>
+      <c r="F2" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="56.25" customHeight="1">
+      <c r="A3" s="65"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="72" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>8</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="14.1" customHeight="1">
-      <c r="A3" s="47"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>10</v>
       </c>
       <c r="G3" s="12"/>
     </row>
@@ -8098,18 +8096,18 @@
       <c r="A4" s="14">
         <v>12</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="12"/>
     </row>
@@ -8117,18 +8115,18 @@
       <c r="A5" s="14">
         <v>15</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="45"/>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="8" t="s">
+      <c r="F5" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>17</v>
       </c>
       <c r="G5" s="12"/>
     </row>
@@ -8136,37 +8134,37 @@
       <c r="A6" s="14">
         <v>16</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="45"/>
+      <c r="D6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="24" customHeight="1">
       <c r="A7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="45"/>
+      <c r="D7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="E7" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G7" s="2"/>
     </row>
@@ -8174,18 +8172,18 @@
       <c r="A8" s="17">
         <v>1020</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="45"/>
+      <c r="D8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="8" t="s">
+      <c r="F8" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>28</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -8193,1495 +8191,1495 @@
       <c r="A9" s="17">
         <v>1030</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="45"/>
+      <c r="D9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="53"/>
-      <c r="D9" s="8" t="s">
+      <c r="F9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="51.95" customHeight="1">
+      <c r="A10" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="B10" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="51.95" customHeight="1">
-      <c r="A10" s="54" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="E10" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50" t="s">
+      <c r="F10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" ht="41.1" customHeight="1">
+      <c r="A11" s="59"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" ht="41.1" customHeight="1">
-      <c r="A11" s="55"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="8" t="s">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="32.1" customHeight="1">
+      <c r="A12" s="64">
+        <v>50</v>
+      </c>
+      <c r="B12" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="32.1" customHeight="1">
-      <c r="A12" s="46">
+      <c r="E12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" ht="42.95" customHeight="1">
+      <c r="A13" s="68"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="21.95" customHeight="1">
+      <c r="A14" s="68"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="51" customHeight="1">
+      <c r="A15" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="69" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="12" customHeight="1">
+      <c r="A16" s="59"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="12.6" customHeight="1">
+      <c r="A17" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="11" t="s">
+      <c r="F17" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1">
+      <c r="A18" s="60"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" ht="42.95" customHeight="1">
-      <c r="A13" s="56"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="8" t="s">
+    </row>
+    <row r="19" spans="1:6" ht="14.1" customHeight="1">
+      <c r="A19" s="60"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="21.95" customHeight="1">
-      <c r="A14" s="56"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" ht="51" customHeight="1">
-      <c r="A15" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="57" t="s">
+      <c r="F19" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="62.1" customHeight="1">
+      <c r="A20" s="59"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A21" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="21" t="s">
+      <c r="F21" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="69.95" customHeight="1">
+      <c r="A22" s="60"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F22" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="12" customHeight="1">
-      <c r="A16" s="55"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="12.6" customHeight="1">
-      <c r="A17" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
-      <c r="A18" s="61"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.1" customHeight="1">
-      <c r="A19" s="61"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="62.1" customHeight="1">
-      <c r="A20" s="55"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="45"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A21" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="59" t="s">
+    </row>
+    <row r="23" spans="1:6" ht="12" customHeight="1">
+      <c r="A23" s="59"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="11" t="s">
+      <c r="F23" s="13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="69.95" customHeight="1">
-      <c r="A22" s="61"/>
-      <c r="B22" s="57"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="12" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="8" t="s">
+    <row r="24" spans="1:6" ht="12.95" customHeight="1">
+      <c r="A24" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="B24" s="46" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="12.95" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="C24" s="47"/>
+      <c r="D24" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="48" t="s">
+      <c r="E24" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="59" t="s">
+    </row>
+    <row r="25" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A25" s="59"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E24" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="F25" s="13" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A25" s="55"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60.95" customHeight="1">
       <c r="A26" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="E26" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="49"/>
-      <c r="D26" s="19" t="s">
+      <c r="F26" s="24" t="s">
         <v>77</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="24" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="21.95" customHeight="1">
       <c r="A27" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="43"/>
+      <c r="D27" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="44" t="s">
+      <c r="E27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="6" t="s">
+      <c r="F27" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="23.1" customHeight="1">
       <c r="A28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="45"/>
+      <c r="D28" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="52" t="s">
+      <c r="E28" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="8" t="s">
+      <c r="F28" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="60.95" customHeight="1">
       <c r="A29" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="45"/>
+      <c r="D29" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="52" t="s">
+      <c r="E29" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="53"/>
-      <c r="D29" s="8" t="s">
+      <c r="F29" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="21.95" customHeight="1">
       <c r="A30" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="45"/>
+      <c r="D30" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="E30" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="53"/>
-      <c r="D30" s="8" t="s">
+      <c r="F30" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="51" customHeight="1">
       <c r="A31" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="45"/>
+      <c r="D31" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="B31" s="52" t="s">
+      <c r="E31" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C31" s="53"/>
-      <c r="D31" s="8" t="s">
+      <c r="F31" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="14">
         <v>70</v>
       </c>
-      <c r="B32" s="52" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" s="53"/>
+      <c r="B32" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="45"/>
       <c r="D32" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.1" customHeight="1">
+      <c r="A33" s="64">
+        <v>71</v>
+      </c>
+      <c r="B33" s="46" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="47"/>
+      <c r="D33" s="48" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="14.1" customHeight="1">
-      <c r="A33" s="46">
-        <v>71</v>
-      </c>
-      <c r="B33" s="48" t="s">
+      <c r="E33" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50" t="s">
+      <c r="F33" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="8" t="s">
+    </row>
+    <row r="34" spans="1:6" ht="72" customHeight="1">
+      <c r="A34" s="68"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F33" s="13" t="s">
+      <c r="F34" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="72" customHeight="1">
-      <c r="A34" s="56"/>
-      <c r="B34" s="57"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>113</v>
-      </c>
-    </row>
     <row r="35" spans="1:6" ht="71.099999999999994" customHeight="1">
-      <c r="A35" s="47"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="51"/>
+      <c r="A35" s="65"/>
+      <c r="B35" s="42"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="61"/>
       <c r="E35" s="15"/>
       <c r="F35" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="72" customHeight="1">
+      <c r="A36" s="64">
+        <v>72</v>
+      </c>
+      <c r="B36" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="47"/>
+      <c r="D36" s="66" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="72" customHeight="1">
-      <c r="A36" s="46">
-        <v>72</v>
-      </c>
-      <c r="B36" s="48" t="s">
+      <c r="E36" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="59" t="s">
+      <c r="F36" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="15" t="s">
+    </row>
+    <row r="37" spans="1:6" ht="101.1" customHeight="1">
+      <c r="A37" s="68"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F37" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="101.1" customHeight="1">
-      <c r="A37" s="56"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="10" t="s">
+    <row r="38" spans="1:6" ht="69.95" customHeight="1">
+      <c r="A38" s="68">
+        <v>73</v>
+      </c>
+      <c r="B38" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="C38" s="53"/>
+      <c r="D38" s="69" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="69.95" customHeight="1">
-      <c r="A38" s="56">
-        <v>73</v>
-      </c>
-      <c r="B38" s="57" t="s">
+      <c r="E38" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="60" t="s">
+    </row>
+    <row r="39" spans="1:6" ht="23.1" customHeight="1">
+      <c r="A39" s="65"/>
+      <c r="B39" s="42"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F39" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="23.1" customHeight="1">
-      <c r="A39" s="47"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="21.95" customHeight="1">
       <c r="A40" s="14">
         <v>74</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="45"/>
+      <c r="D40" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="D40" s="8" t="s">
+      <c r="F40" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="E40" s="8" t="s">
+    </row>
+    <row r="41" spans="1:6" ht="24" customHeight="1">
+      <c r="A41" s="64">
+        <v>75</v>
+      </c>
+      <c r="B41" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="C41" s="47"/>
+      <c r="D41" s="48" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="24" customHeight="1">
-      <c r="A41" s="46">
-        <v>75</v>
-      </c>
-      <c r="B41" s="48" t="s">
+      <c r="E41" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="49"/>
-      <c r="D41" s="50" t="s">
+      <c r="F41" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="42" spans="1:6" ht="41.1" customHeight="1">
-      <c r="A42" s="47"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="45"/>
-      <c r="D42" s="51"/>
+      <c r="A42" s="65"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="43"/>
+      <c r="D42" s="61"/>
       <c r="E42" s="15"/>
       <c r="F42" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A43" s="64">
+        <v>77</v>
+      </c>
+      <c r="B43" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="66" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A43" s="46">
-        <v>77</v>
-      </c>
-      <c r="B43" s="48" t="s">
+      <c r="E43" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C43" s="49"/>
-      <c r="D43" s="59" t="s">
+    </row>
+    <row r="44" spans="1:6" ht="31.5" customHeight="1">
+      <c r="A44" s="65"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F44" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="15" t="s">
+    </row>
+    <row r="45" spans="1:6" ht="15" customHeight="1">
+      <c r="A45" s="64">
+        <v>78</v>
+      </c>
+      <c r="B45" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C45" s="47"/>
+      <c r="D45" s="66" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="14.1" customHeight="1">
+      <c r="A46" s="65"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="67"/>
+      <c r="E46" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="F43" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="31.5" customHeight="1">
-      <c r="A44" s="47"/>
-      <c r="B44" s="44"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1">
-      <c r="A45" s="46">
-        <v>78</v>
-      </c>
-      <c r="B45" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="59" t="s">
+      <c r="F46" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="14.1" customHeight="1">
-      <c r="A46" s="47"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="51" customHeight="1">
       <c r="A47" s="14">
         <v>79</v>
       </c>
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C47" s="45"/>
+      <c r="D47" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="C47" s="53"/>
-      <c r="D47" s="8" t="s">
+      <c r="F47" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="32.1" customHeight="1">
       <c r="A48" s="14">
         <v>80</v>
       </c>
-      <c r="B48" s="52" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" s="53"/>
+      <c r="B48" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C48" s="45"/>
       <c r="D48" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="80.099999999999994" customHeight="1">
       <c r="A49" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="45"/>
+      <c r="D49" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="E49" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="53"/>
-      <c r="D49" s="8" t="s">
+      <c r="F49" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="E49" s="8" t="s">
+    </row>
+    <row r="50" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A50" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="B50" s="46" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A50" s="54" t="s">
+      <c r="C50" s="47"/>
+      <c r="D50" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="48" t="s">
+      <c r="E50" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="50" t="s">
+      <c r="F50" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="E50" s="8" t="s">
+    </row>
+    <row r="51" spans="1:6" ht="39.950000000000003" customHeight="1">
+      <c r="A51" s="60"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F51" s="9" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="39.950000000000003" customHeight="1">
-      <c r="A51" s="61"/>
-      <c r="B51" s="57"/>
-      <c r="C51" s="58"/>
-      <c r="D51" s="63"/>
-      <c r="E51" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="51" customHeight="1">
       <c r="A52" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="43"/>
+      <c r="D52" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B52" s="44" t="s">
+      <c r="E52" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="C52" s="45"/>
-      <c r="D52" s="6" t="s">
+      <c r="F52" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>164</v>
-      </c>
-      <c r="F52" s="22" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="32.1" customHeight="1">
       <c r="A53" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C53" s="45"/>
+      <c r="D53" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="E53" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="8" t="s">
+      <c r="F53" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="E53" s="8" t="s">
+    </row>
+    <row r="54" spans="1:6" ht="51" customHeight="1">
+      <c r="A54" s="58" t="s">
         <v>169</v>
       </c>
-      <c r="F53" s="11" t="s">
+      <c r="B54" s="46" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="51" customHeight="1">
-      <c r="A54" s="54" t="s">
+      <c r="C54" s="47"/>
+      <c r="D54" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="B54" s="48" t="s">
+      <c r="E54" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C54" s="49"/>
-      <c r="D54" s="15" t="s">
+      <c r="F54" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="E54" s="8" t="s">
+    </row>
+    <row r="55" spans="1:6" ht="32.1" customHeight="1">
+      <c r="A55" s="60"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="F54" s="13" t="s">
+      <c r="E55" s="15" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="32.1" customHeight="1">
-      <c r="A55" s="61"/>
-      <c r="B55" s="57"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="8" t="s">
+      <c r="F55" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="E55" s="15" t="s">
+    </row>
+    <row r="56" spans="1:6" ht="108" customHeight="1">
+      <c r="A56" s="60"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="53"/>
+      <c r="D56" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="E56" s="8" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="108" customHeight="1">
-      <c r="A56" s="61"/>
-      <c r="B56" s="57"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="8" t="s">
+      <c r="F56" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="E56" s="8" t="s">
+    </row>
+    <row r="57" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A57" s="60"/>
+      <c r="B57" s="52"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="63"/>
+      <c r="F57" s="24" t="s">
         <v>180</v>
       </c>
-      <c r="F56" s="11" t="s">
+    </row>
+    <row r="58" spans="1:6" ht="51.95" customHeight="1">
+      <c r="A58" s="60" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A57" s="61"/>
-      <c r="B57" s="57"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="64"/>
-      <c r="E57" s="65"/>
-      <c r="F57" s="24" t="s">
+      <c r="B58" s="52" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="51.95" customHeight="1">
-      <c r="A58" s="61" t="s">
+      <c r="C58" s="53"/>
+      <c r="D58" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B58" s="57" t="s">
+      <c r="E58" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="C58" s="58"/>
-      <c r="D58" s="6" t="s">
+      <c r="F58" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="59" spans="1:6" ht="12.95" customHeight="1">
-      <c r="A59" s="61"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="58"/>
+      <c r="A59" s="60"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="53"/>
       <c r="D59" s="15"/>
       <c r="E59" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="30.95" customHeight="1">
+      <c r="A60" s="60"/>
+      <c r="B60" s="52"/>
+      <c r="C60" s="53"/>
+      <c r="D60" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="E60" s="8" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" ht="30.95" customHeight="1">
-      <c r="A60" s="61"/>
-      <c r="B60" s="57"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="50" t="s">
+      <c r="F60" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="E60" s="8" t="s">
+    </row>
+    <row r="61" spans="1:6" ht="15" customHeight="1">
+      <c r="A61" s="60"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="53"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F61" s="13" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15" customHeight="1">
-      <c r="A61" s="61"/>
-      <c r="B61" s="57"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="63"/>
-      <c r="E61" s="8" t="s">
+    <row r="62" spans="1:6" ht="14.1" customHeight="1">
+      <c r="A62" s="60"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F62" s="13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="62.1" customHeight="1">
+      <c r="A63" s="60"/>
+      <c r="B63" s="52"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="8" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" ht="14.1" customHeight="1">
-      <c r="A62" s="61"/>
-      <c r="B62" s="57"/>
-      <c r="C62" s="58"/>
-      <c r="D62" s="63"/>
-      <c r="E62" s="8" t="s">
+      <c r="F63" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="F62" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="62.1" customHeight="1">
-      <c r="A63" s="61"/>
-      <c r="B63" s="57"/>
-      <c r="C63" s="58"/>
-      <c r="D63" s="51"/>
-      <c r="E63" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="F63" s="13" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="64" spans="1:6" ht="42" customHeight="1">
-      <c r="A64" s="55"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="67"/>
+      <c r="A64" s="59"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="51"/>
       <c r="F64" s="11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="50.1" customHeight="1">
       <c r="A65" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="B65" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" s="45"/>
+      <c r="D65" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="B65" s="52" t="s">
+      <c r="E65" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="C65" s="53"/>
-      <c r="D65" s="8" t="s">
+      <c r="F65" s="13" t="s">
         <v>200</v>
-      </c>
-      <c r="E65" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F65" s="13" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="119.1" customHeight="1">
       <c r="A66" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B66" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="C66" s="45"/>
+      <c r="D66" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B66" s="52" t="s">
+      <c r="E66" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="C66" s="53"/>
-      <c r="D66" s="8" t="s">
+      <c r="F66" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="128.1" customHeight="1">
       <c r="A67" s="14">
         <v>105</v>
       </c>
-      <c r="B67" s="52" t="s">
-        <v>208</v>
-      </c>
-      <c r="C67" s="53"/>
+      <c r="B67" s="44" t="s">
+        <v>206</v>
+      </c>
+      <c r="C67" s="45"/>
       <c r="D67" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E67" s="27"/>
       <c r="F67" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="58.7" customHeight="1">
       <c r="A68" s="14">
         <v>107</v>
       </c>
-      <c r="B68" s="52" t="s">
+      <c r="B68" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="45"/>
+      <c r="D68" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C68" s="53"/>
-      <c r="D68" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>213</v>
-      </c>
       <c r="F68" s="13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1">
       <c r="A69" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="C69" s="45"/>
+      <c r="D69" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B69" s="52" t="s">
+      <c r="E69" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="C69" s="53"/>
-      <c r="D69" s="8" t="s">
+      <c r="F69" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.1" customHeight="1">
       <c r="A70" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="C70" s="45"/>
+      <c r="D70" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="B70" s="52" t="s">
+      <c r="E70" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="C70" s="53"/>
-      <c r="D70" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>222</v>
-      </c>
       <c r="F70" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="21.95" customHeight="1">
       <c r="A71" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="B71" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="C71" s="45"/>
+      <c r="D71" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B71" s="52" t="s">
+      <c r="E71" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C71" s="53"/>
-      <c r="D71" s="8" t="s">
+      <c r="F71" s="11" t="s">
         <v>225</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="110.1" customHeight="1">
       <c r="A72" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" s="44" t="s">
+        <v>227</v>
+      </c>
+      <c r="C72" s="45"/>
+      <c r="D72" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="B72" s="52" t="s">
+      <c r="E72" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="C72" s="53"/>
-      <c r="D72" s="8" t="s">
+      <c r="F72" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="E72" s="8" t="s">
+    </row>
+    <row r="73" spans="1:6" ht="12" customHeight="1">
+      <c r="A73" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="F72" s="11" t="s">
+      <c r="B73" s="46" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" ht="12" customHeight="1">
-      <c r="A73" s="54" t="s">
+      <c r="C73" s="47"/>
+      <c r="D73" s="48" t="s">
         <v>233</v>
       </c>
-      <c r="B73" s="48" t="s">
+      <c r="E73" s="8" t="s">
         <v>234</v>
       </c>
-      <c r="C73" s="49"/>
-      <c r="D73" s="50" t="s">
+      <c r="F73" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="E73" s="8" t="s">
+    </row>
+    <row r="74" spans="1:6" ht="21.95" customHeight="1">
+      <c r="A74" s="60"/>
+      <c r="B74" s="52"/>
+      <c r="C74" s="53"/>
+      <c r="D74" s="49"/>
+      <c r="E74" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="F73" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="21.95" customHeight="1">
-      <c r="A74" s="61"/>
-      <c r="B74" s="57"/>
-      <c r="C74" s="58"/>
-      <c r="D74" s="63"/>
-      <c r="E74" s="19" t="s">
-        <v>238</v>
-      </c>
       <c r="F74" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="12.95" customHeight="1">
       <c r="A75" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B75" s="42" t="s">
+        <v>238</v>
+      </c>
+      <c r="C75" s="43"/>
+      <c r="D75" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="B75" s="44" t="s">
+      <c r="E75" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C75" s="45"/>
-      <c r="D75" s="6" t="s">
+      <c r="F75" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="21.95" customHeight="1">
       <c r="A76" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B76" s="44" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="45"/>
+      <c r="D76" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="B76" s="52" t="s">
+      <c r="E76" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C76" s="53"/>
-      <c r="D76" s="8" t="s">
+      <c r="F76" s="13" t="s">
         <v>246</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="F76" s="13" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="59.1" customHeight="1">
       <c r="A77" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="B77" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="C77" s="45"/>
+      <c r="D77" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="B77" s="52" t="s">
+      <c r="E77" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="C77" s="53"/>
-      <c r="D77" s="8" t="s">
+      <c r="F77" s="11" t="s">
         <v>251</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="69.95" customHeight="1">
       <c r="A78" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="B78" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="C78" s="45"/>
+      <c r="D78" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="B78" s="52" t="s">
+      <c r="E78" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="C78" s="53"/>
-      <c r="D78" s="8" t="s">
+      <c r="F78" s="11" t="s">
         <v>256</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="32.1" customHeight="1">
       <c r="A79" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="B79" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C79" s="45"/>
+      <c r="D79" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="B79" s="52" t="s">
+      <c r="E79" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="C79" s="53"/>
-      <c r="D79" s="8" t="s">
+      <c r="F79" s="13" t="s">
         <v>261</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="F79" s="13" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="12.95" customHeight="1">
       <c r="A80" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="B80" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="C80" s="45"/>
+      <c r="D80" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="B80" s="52" t="s">
+      <c r="E80" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="C80" s="53"/>
-      <c r="D80" s="8" t="s">
+      <c r="F80" s="11" t="s">
         <v>266</v>
-      </c>
-      <c r="E80" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="F80" s="11" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="32.1" customHeight="1">
       <c r="A81" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="B81" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="C81" s="45"/>
+      <c r="D81" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="B81" s="52" t="s">
+      <c r="E81" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C81" s="53"/>
-      <c r="D81" s="8" t="s">
+      <c r="F81" s="11" t="s">
         <v>271</v>
-      </c>
-      <c r="E81" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="F81" s="11" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="32.1" customHeight="1">
       <c r="A82" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B82" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82" s="45"/>
+      <c r="D82" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="B82" s="52" t="s">
+      <c r="E82" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="C82" s="53"/>
-      <c r="D82" s="8" t="s">
+      <c r="F82" s="11" t="s">
         <v>276</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="F82" s="11" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="32.1" customHeight="1">
       <c r="A83" s="28" t="s">
+        <v>277</v>
+      </c>
+      <c r="B83" s="46" t="s">
+        <v>278</v>
+      </c>
+      <c r="C83" s="47"/>
+      <c r="D83" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="B83" s="48" t="s">
+      <c r="E83" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="C83" s="49"/>
-      <c r="D83" s="10" t="s">
+      <c r="F83" s="24" t="s">
         <v>281</v>
-      </c>
-      <c r="E83" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="F83" s="24" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="33" customHeight="1">
       <c r="A84" s="25" t="s">
+        <v>282</v>
+      </c>
+      <c r="B84" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="C84" s="43"/>
+      <c r="D84" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="B84" s="44" t="s">
+      <c r="E84" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C84" s="45"/>
-      <c r="D84" s="6" t="s">
+      <c r="F84" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="E84" s="6" t="s">
+    </row>
+    <row r="85" spans="1:6" ht="32.1" customHeight="1">
+      <c r="A85" s="58" t="s">
         <v>287</v>
       </c>
-      <c r="F84" s="22" t="s">
+      <c r="B85" s="46" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" ht="32.1" customHeight="1">
-      <c r="A85" s="54" t="s">
+      <c r="C85" s="47"/>
+      <c r="D85" s="48" t="s">
         <v>289</v>
       </c>
-      <c r="B85" s="48" t="s">
+      <c r="E85" s="8" t="s">
         <v>290</v>
       </c>
-      <c r="C85" s="49"/>
-      <c r="D85" s="50" t="s">
+      <c r="F85" s="11" t="s">
         <v>291</v>
       </c>
-      <c r="E85" s="8" t="s">
+    </row>
+    <row r="86" spans="1:6" ht="41.1" customHeight="1">
+      <c r="A86" s="60"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="53"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="8" t="s">
         <v>292</v>
       </c>
-      <c r="F85" s="11" t="s">
+      <c r="F86" s="11" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="41.1" customHeight="1">
-      <c r="A86" s="61"/>
-      <c r="B86" s="57"/>
-      <c r="C86" s="58"/>
-      <c r="D86" s="63"/>
-      <c r="E86" s="8" t="s">
+    <row r="87" spans="1:6" ht="31.35" customHeight="1">
+      <c r="A87" s="59"/>
+      <c r="B87" s="42"/>
+      <c r="C87" s="43"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="F86" s="11" t="s">
+      <c r="F87" s="11" t="s">
         <v>295</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="31.35" customHeight="1">
-      <c r="A87" s="55"/>
-      <c r="B87" s="44"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="51"/>
-      <c r="E87" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1">
       <c r="A88" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B88" s="46" t="s">
+        <v>297</v>
+      </c>
+      <c r="C88" s="47"/>
+      <c r="D88" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="B88" s="48" t="s">
+      <c r="E88" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="C88" s="49"/>
-      <c r="D88" s="10" t="s">
+      <c r="F88" s="24" t="s">
         <v>300</v>
-      </c>
-      <c r="E88" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="F88" s="24" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.1" customHeight="1">
       <c r="A89" s="29" t="s">
+        <v>301</v>
+      </c>
+      <c r="B89" s="52" t="s">
+        <v>302</v>
+      </c>
+      <c r="C89" s="53"/>
+      <c r="D89" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="B89" s="57" t="s">
+      <c r="E89" s="6" t="s">
         <v>304</v>
-      </c>
-      <c r="C89" s="58"/>
-      <c r="D89" s="23" t="s">
-        <v>305</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="F89" s="22"/>
     </row>
     <row r="90" spans="1:6" ht="51" customHeight="1">
       <c r="A90" s="30"/>
-      <c r="B90" s="68"/>
-      <c r="C90" s="69"/>
+      <c r="B90" s="54"/>
+      <c r="C90" s="56"/>
       <c r="D90" s="20"/>
       <c r="E90" s="15" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="50.1" customHeight="1">
       <c r="A91" s="30"/>
-      <c r="B91" s="68"/>
-      <c r="C91" s="69"/>
+      <c r="B91" s="54"/>
+      <c r="C91" s="56"/>
       <c r="D91" s="20"/>
       <c r="E91" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="72" customHeight="1">
       <c r="A92" s="30"/>
-      <c r="B92" s="68"/>
-      <c r="C92" s="69"/>
+      <c r="B92" s="54"/>
+      <c r="C92" s="56"/>
       <c r="D92" s="20"/>
       <c r="E92" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="89.1" customHeight="1">
       <c r="A93" s="30"/>
-      <c r="B93" s="68"/>
-      <c r="C93" s="69"/>
+      <c r="B93" s="54"/>
+      <c r="C93" s="56"/>
       <c r="D93" s="20"/>
       <c r="E93" s="15" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F93" s="11" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="51" customHeight="1">
       <c r="A94" s="31"/>
-      <c r="B94" s="70"/>
-      <c r="C94" s="71"/>
+      <c r="B94" s="55"/>
+      <c r="C94" s="57"/>
       <c r="D94" s="21"/>
       <c r="E94" s="15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="80.099999999999994" customHeight="1">
       <c r="A95" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="B95" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="C95" s="45"/>
+      <c r="D95" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B95" s="52" t="s">
+      <c r="E95" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="C95" s="53"/>
-      <c r="D95" s="8" t="s">
+      <c r="F95" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="E95" s="8" t="s">
+    </row>
+    <row r="96" spans="1:6" ht="89.1" customHeight="1">
+      <c r="A96" s="58" t="s">
         <v>320</v>
       </c>
-      <c r="F95" s="11" t="s">
+      <c r="B96" s="46" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" ht="89.1" customHeight="1">
-      <c r="A96" s="54" t="s">
+      <c r="C96" s="47"/>
+      <c r="D96" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="B96" s="48" t="s">
+      <c r="E96" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="C96" s="49"/>
-      <c r="D96" s="8" t="s">
+      <c r="F96" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="E96" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="F96" s="11" t="s">
-        <v>326</v>
-      </c>
     </row>
     <row r="97" spans="1:6" ht="51.95" customHeight="1">
-      <c r="A97" s="55"/>
-      <c r="B97" s="44"/>
-      <c r="C97" s="45"/>
+      <c r="A97" s="59"/>
+      <c r="B97" s="42"/>
+      <c r="C97" s="43"/>
       <c r="D97" s="26"/>
       <c r="E97" s="15" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="80.45" customHeight="1">
       <c r="A98" s="16" t="s">
+        <v>326</v>
+      </c>
+      <c r="B98" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="C98" s="45"/>
+      <c r="D98" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="B98" s="52" t="s">
+      <c r="E98" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="C98" s="53"/>
-      <c r="D98" s="8" t="s">
-        <v>330</v>
-      </c>
-      <c r="E98" s="15" t="s">
-        <v>331</v>
-      </c>
       <c r="F98" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="15" customHeight="1">
       <c r="A99" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="B99" s="46" t="s">
+        <v>331</v>
+      </c>
+      <c r="C99" s="47"/>
+      <c r="D99" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="B99" s="48" t="s">
+      <c r="E99" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="C99" s="49"/>
-      <c r="D99" s="10" t="s">
+      <c r="F99" s="24" t="s">
         <v>334</v>
-      </c>
-      <c r="E99" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F99" s="24" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="14.1" customHeight="1">
       <c r="A100" s="32">
         <v>201</v>
       </c>
-      <c r="B100" s="57" t="s">
+      <c r="B100" s="52" t="s">
+        <v>335</v>
+      </c>
+      <c r="C100" s="53"/>
+      <c r="D100" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="E100" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="C100" s="58"/>
-      <c r="D100" s="23" t="s">
+      <c r="F100" s="54" t="s">
         <v>338</v>
-      </c>
-      <c r="E100" s="23" t="s">
-        <v>339</v>
-      </c>
-      <c r="F100" s="68" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="81" customHeight="1">
       <c r="A101" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="B101" s="57" t="s">
-        <v>341</v>
-      </c>
-      <c r="C101" s="58"/>
+        <v>339</v>
+      </c>
+      <c r="B101" s="52" t="s">
+        <v>339</v>
+      </c>
+      <c r="C101" s="53"/>
       <c r="D101" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E101" s="34"/>
-      <c r="F101" s="68"/>
+      <c r="F101" s="54"/>
     </row>
     <row r="102" spans="1:6" ht="81" customHeight="1">
       <c r="A102" s="35">
         <v>208</v>
       </c>
-      <c r="B102" s="44" t="s">
-        <v>342</v>
-      </c>
-      <c r="C102" s="45"/>
+      <c r="B102" s="42" t="s">
+        <v>340</v>
+      </c>
+      <c r="C102" s="43"/>
       <c r="D102" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E102" s="21"/>
-      <c r="F102" s="70"/>
+      <c r="F102" s="55"/>
     </row>
     <row r="103" spans="1:6" ht="101.1" customHeight="1">
       <c r="A103" s="14">
         <v>209</v>
       </c>
-      <c r="B103" s="52" t="s">
+      <c r="B103" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="C103" s="45"/>
+      <c r="D103" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="E103" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="C103" s="53"/>
-      <c r="D103" s="8" t="s">
+      <c r="F103" s="9" t="s">
         <v>345</v>
-      </c>
-      <c r="E103" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="51" customHeight="1">
       <c r="A104" s="14">
         <v>210</v>
       </c>
-      <c r="B104" s="66" t="s">
-        <v>348</v>
-      </c>
-      <c r="C104" s="67"/>
+      <c r="B104" s="50" t="s">
+        <v>346</v>
+      </c>
+      <c r="C104" s="51"/>
       <c r="D104" s="8" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E104" s="34"/>
       <c r="F104" s="36"/>
@@ -9690,26 +9688,26 @@
       <c r="A105" s="37">
         <v>211</v>
       </c>
-      <c r="B105" s="48" t="s">
-        <v>350</v>
-      </c>
-      <c r="C105" s="49"/>
+      <c r="B105" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="C105" s="47"/>
       <c r="D105" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E105" s="38"/>
       <c r="F105" s="39"/>
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1">
       <c r="A106" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="B106" s="57" t="s">
-        <v>341</v>
-      </c>
-      <c r="C106" s="58"/>
+        <v>339</v>
+      </c>
+      <c r="B106" s="52" t="s">
+        <v>339</v>
+      </c>
+      <c r="C106" s="53"/>
       <c r="D106" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E106" s="38"/>
       <c r="F106" s="39"/>
@@ -9718,12 +9716,12 @@
       <c r="A107" s="32">
         <v>218</v>
       </c>
-      <c r="B107" s="57" t="s">
-        <v>352</v>
-      </c>
-      <c r="C107" s="58"/>
+      <c r="B107" s="52" t="s">
+        <v>350</v>
+      </c>
+      <c r="C107" s="53"/>
       <c r="D107" s="23" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E107" s="38"/>
       <c r="F107" s="39"/>
@@ -9732,237 +9730,237 @@
       <c r="A108" s="35">
         <v>219</v>
       </c>
-      <c r="B108" s="44" t="s">
+      <c r="B108" s="42" t="s">
+        <v>352</v>
+      </c>
+      <c r="C108" s="43"/>
+      <c r="D108" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="F108" s="22" t="s">
         <v>354</v>
-      </c>
-      <c r="C108" s="45"/>
-      <c r="D108" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>339</v>
-      </c>
-      <c r="F108" s="22" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="51.95" customHeight="1">
       <c r="A109" s="14">
         <v>220</v>
       </c>
-      <c r="B109" s="52" t="s">
+      <c r="B109" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="C109" s="45"/>
+      <c r="D109" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E109" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C109" s="53"/>
-      <c r="D109" s="8" t="s">
+      <c r="F109" s="11" t="s">
         <v>358</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="F109" s="11" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="51.95" customHeight="1">
       <c r="A110" s="16" t="s">
+        <v>359</v>
+      </c>
+      <c r="B110" s="44" t="s">
+        <v>360</v>
+      </c>
+      <c r="C110" s="45"/>
+      <c r="D110" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="B110" s="52" t="s">
+      <c r="E110" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="C110" s="53"/>
-      <c r="D110" s="8" t="s">
+      <c r="F110" s="13" t="s">
         <v>363</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="F110" s="13" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="69.95" customHeight="1">
       <c r="A111" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="B111" s="44" t="s">
+        <v>365</v>
+      </c>
+      <c r="C111" s="45"/>
+      <c r="D111" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="B111" s="52" t="s">
+      <c r="E111" s="8" t="s">
         <v>367</v>
       </c>
-      <c r="C111" s="53"/>
-      <c r="D111" s="8" t="s">
+      <c r="F111" s="13" t="s">
         <v>368</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>369</v>
-      </c>
-      <c r="F111" s="13" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="60.95" customHeight="1">
       <c r="A112" s="14">
         <v>230</v>
       </c>
-      <c r="B112" s="66" t="s">
+      <c r="B112" s="50" t="s">
+        <v>369</v>
+      </c>
+      <c r="C112" s="51"/>
+      <c r="D112" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="E112" s="8" t="s">
         <v>371</v>
       </c>
-      <c r="C112" s="67"/>
-      <c r="D112" s="8" t="s">
+      <c r="F112" s="13" t="s">
         <v>372</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="F112" s="13" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="60.95" customHeight="1">
       <c r="A113" s="14">
         <v>231</v>
       </c>
-      <c r="B113" s="52" t="s">
+      <c r="B113" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="C113" s="45"/>
+      <c r="D113" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="E113" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="C113" s="53"/>
-      <c r="D113" s="8" t="s">
+      <c r="F113" s="11" t="s">
         <v>376</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="F113" s="11" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="71.099999999999994" customHeight="1">
       <c r="A114" s="14">
         <v>232</v>
       </c>
-      <c r="B114" s="52" t="s">
+      <c r="B114" s="44" t="s">
+        <v>377</v>
+      </c>
+      <c r="C114" s="45"/>
+      <c r="D114" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="E114" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="C114" s="53"/>
-      <c r="D114" s="8" t="s">
+      <c r="F114" s="11" t="s">
         <v>380</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="F114" s="11" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="41.1" customHeight="1">
       <c r="A115" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="B115" s="44" t="s">
+        <v>382</v>
+      </c>
+      <c r="C115" s="45"/>
+      <c r="D115" s="48" t="s">
         <v>383</v>
       </c>
-      <c r="B115" s="52" t="s">
+      <c r="E115" s="8" t="s">
         <v>384</v>
       </c>
-      <c r="C115" s="53"/>
-      <c r="D115" s="50" t="s">
+      <c r="F115" s="11" t="s">
         <v>385</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="F115" s="11" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="32.1" customHeight="1">
       <c r="A116" s="28" t="s">
+        <v>386</v>
+      </c>
+      <c r="B116" s="46" t="s">
+        <v>387</v>
+      </c>
+      <c r="C116" s="47"/>
+      <c r="D116" s="49"/>
+      <c r="E116" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="B116" s="48" t="s">
+      <c r="F116" s="9" t="s">
         <v>389</v>
-      </c>
-      <c r="C116" s="49"/>
-      <c r="D116" s="63"/>
-      <c r="E116" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="51" customHeight="1">
       <c r="A117" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="B117" s="42" t="s">
+        <v>391</v>
+      </c>
+      <c r="C117" s="43"/>
+      <c r="D117" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="B117" s="44" t="s">
+      <c r="E117" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="C117" s="45"/>
-      <c r="D117" s="6" t="s">
+      <c r="F117" s="22" t="s">
         <v>394</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="F117" s="22" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="61.5" customHeight="1">
       <c r="A118" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="B118" s="44" t="s">
+        <v>396</v>
+      </c>
+      <c r="C118" s="45"/>
+      <c r="D118" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E118" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="B118" s="52" t="s">
+      <c r="F118" s="13" t="s">
         <v>398</v>
-      </c>
-      <c r="C118" s="53"/>
-      <c r="D118" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="F118" s="13" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="15" customHeight="1">
       <c r="A119" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="B119" s="44" t="s">
+        <v>400</v>
+      </c>
+      <c r="C119" s="45"/>
+      <c r="D119" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E119" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="B119" s="52" t="s">
+      <c r="F119" s="13" t="s">
         <v>402</v>
-      </c>
-      <c r="C119" s="53"/>
-      <c r="D119" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="E119" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="F119" s="13" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="14.1" customHeight="1">
       <c r="A120" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="B120" s="46" t="s">
+        <v>404</v>
+      </c>
+      <c r="C120" s="47"/>
+      <c r="D120" s="10" t="s">
         <v>405</v>
       </c>
-      <c r="B120" s="48" t="s">
+      <c r="E120" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="C120" s="49"/>
-      <c r="D120" s="10" t="s">
+      <c r="F120" s="24" t="s">
         <v>407</v>
-      </c>
-      <c r="E120" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="F120" s="24" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="36.950000000000003" customHeight="1">
       <c r="A121" s="40" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B121" s="40"/>
       <c r="C121" s="40"/>
@@ -10027,115 +10025,10 @@
     <row r="150" spans="7:7" ht="12.6" customHeight="1"/>
   </sheetData>
   <mergeCells count="128">
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:D116"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="F100:F102"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="B85:C87"/>
-    <mergeCell ref="D85:D87"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="A58:A64"/>
-    <mergeCell ref="B58:C64"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="A54:A57"/>
-    <mergeCell ref="B54:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:C20"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="B12:C14"/>
     <mergeCell ref="D12:D14"/>
@@ -10151,10 +10044,115 @@
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:C20"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:C23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="B54:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="B58:C64"/>
+    <mergeCell ref="D60:D63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D85:D87"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="B85:C87"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="F100:F102"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="B116:C116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>